<commit_message>
fix read of mappings file
</commit_message>
<xml_diff>
--- a/Simple.xlsx
+++ b/Simple.xlsx
@@ -1,48 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15" conformance="strict">
-  <fileVersion lowestEdited="5" appName="xl" rupBuild="14420" lastEdited="6"/>
-  <workbookPr dateCompatibility="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<zdef1859688791:workbook xmlns="" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:zdef1859688791="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15" conformance="strict">
+  <zdef1859688791:fileVersion xmlns="" lowestEdited="5" appName="xl" rupBuild="14420" lastEdited="6"/>
+  <zdef1859688791:workbookPr xmlns="" dateCompatibility="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\helix.local\data\Home\nickb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <bookViews>
+  <bookViews xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <workbookView xWindow="120" windowHeight="11385" yWindow="465" windowWidth="19020" activeTab="1"/>
   </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet Number 2" sheetId="2" r:id="rId2"/>
+  <sheets xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet Number 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
+  <zdef1859688791:calcPr xmlns="" calcId="152511"/>
+  <extLst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
     </ext>
   </extLst>
-</workbook>
+</zdef1859688791:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="4" uniqueCount="4">
-  <si>
+<zdef-1573754294:sst xmlns="" xmlns:zdef-1573754294="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <t>test</t>
   </si>
-  <si>
+  <si xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <t>test 2</t>
   </si>
-  <si>
+  <si xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <t>This is sheet 2</t>
   </si>
-  <si>
+  <si xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <t>Stuff</t>
   </si>
-</sst>
+</zdef-1573754294:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts x14ac:knownFonts="1" count="1">
     <font>
       <sz val="11"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -378,7 +378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -429,7 +429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">

</xml_diff>

<commit_message>
fix issue with conformance="strict" attribute
</commit_message>
<xml_diff>
--- a/Simple.xlsx
+++ b/Simple.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<zdef1506576592:workbook xmlns="" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:zdef1506576592="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15" conformance="strict">
-  <zdef1506576592:fileVersion xmlns="" lowestEdited="5" appName="xl" rupBuild="14420" lastEdited="6"/>
-  <zdef1506576592:workbookPr xmlns="" dateCompatibility="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion lowestEdited="5" appName="xl" rupBuild="14420" lastEdited="6"/>
+  <workbookPr dateCompatibility="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\helix.local\data\Home\nickb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <bookViews xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <bookViews>
     <workbookView xWindow="120" windowHeight="11385" yWindow="465" windowWidth="19020" activeTab="1"/>
   </bookViews>
-  <sheets xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet Number 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <zdef1506576592:calcPr xmlns="" calcId="152511"/>
-  <extLst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <calcPr calcId="152511"/>
+  <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
     </ext>
   </extLst>
-</zdef1506576592:workbook>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<zdef682147422:sst xmlns="" xmlns:zdef682147422="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<zdef1622804211:sst xmlns="" xmlns:zdef1622804211="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <t>test</t>
   </si>
@@ -38,7 +38,7 @@
   <si xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <t>Stuff</t>
   </si>
-</zdef682147422:sst>
+</zdef1622804211:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
handle more test files and fix issue with expecting all zip entries to be XML
</commit_message>
<xml_diff>
--- a/Simple.xlsx
+++ b/Simple.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<zdef1622804211:sst xmlns="" xmlns:zdef1622804211="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<zdef2053169718:sst xmlns="" xmlns:zdef2053169718="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <t>test</t>
   </si>
@@ -38,7 +38,7 @@
   <si xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <t>Stuff</t>
   </si>
-</zdef1622804211:sst>
+</zdef2053169718:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>